<commit_message>
added support to read Brasil.io files
</commit_message>
<xml_diff>
--- a/assets/SIRD Model.xlsx
+++ b/assets/SIRD Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Task Stage\Task - covidsims\covidsims\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC6520D-2F45-44E2-A5F8-AAEF46B19575}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E799C634-5C0E-4709-9E11-8573304040D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="38640" windowHeight="16440" tabRatio="659" xr2:uid="{C9EED678-3558-4294-B636-EA4BD58922A2}"/>
+    <workbookView xWindow="37830" yWindow="2880" windowWidth="2085" windowHeight="9540" tabRatio="659" xr2:uid="{C9EED678-3558-4294-B636-EA4BD58922A2}"/>
   </bookViews>
   <sheets>
     <sheet name="SIRD model" sheetId="20" r:id="rId1"/>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>https://www.who.int/emergencies/diseases/novel-coronavirus-2019/situation-reports</t>
-  </si>
-  <si>
-    <t>(WHO) Weekly situaltion reports</t>
   </si>
   <si>
     <t>(WHO) Epidemic Intelligence from Open Source</t>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>https://www.viser.com.br/covid-19/sp-covid-info-tracker</t>
+  </si>
+  <si>
+    <t>(WHO) Weekly situation reports</t>
   </si>
 </sst>
 </file>
@@ -8110,18 +8110,18 @@
   <sheetData>
     <row r="7" spans="7:28" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G8" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U8" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
@@ -8133,142 +8133,142 @@
     </row>
     <row r="9" spans="7:28" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="7:28" x14ac:dyDescent="0.25">
       <c r="H10" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U10" t="s">
+        <v>56</v>
+      </c>
+      <c r="V10" t="s">
         <v>57</v>
-      </c>
-      <c r="V10" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11" spans="7:28" x14ac:dyDescent="0.25">
       <c r="H11" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U11" t="s">
+        <v>58</v>
+      </c>
+      <c r="V11" t="s">
         <v>59</v>
-      </c>
-      <c r="V11" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="7:28" x14ac:dyDescent="0.25">
       <c r="H12" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U12" t="s">
+        <v>60</v>
+      </c>
+      <c r="V12" t="s">
         <v>61</v>
-      </c>
-      <c r="V12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="7:28" x14ac:dyDescent="0.25">
       <c r="U13" t="s">
+        <v>73</v>
+      </c>
+      <c r="V13" t="s">
         <v>74</v>
-      </c>
-      <c r="V13" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="15" spans="7:28" x14ac:dyDescent="0.25">
       <c r="U15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="7:28" x14ac:dyDescent="0.25">
       <c r="N16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M17" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V17" t="s">
+        <v>80</v>
+      </c>
+      <c r="W17" t="s">
         <v>81</v>
-      </c>
-      <c r="W17" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W18" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N19" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N20" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N21" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="20" t="s">
-        <v>64</v>
-      </c>
       <c r="H23" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B25" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U25" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
@@ -8280,72 +8280,72 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M29" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="N29" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="N29" s="20" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N31" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N32" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N33" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -12527,23 +12527,23 @@
       </c>
       <c r="E31" s="14">
         <f ca="1">INT(ROUND(_xlfn.NORM.INV(RAND(), $C28,$C31),0))</f>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F31" s="14">
         <f t="shared" ref="F31:AG31" ca="1" si="1">INT(ROUND(_xlfn.NORM.INV(RAND(), $C28,$C31),0))</f>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J31" s="14">
         <f t="shared" ca="1" si="1"/>
@@ -12555,15 +12555,15 @@
       </c>
       <c r="L31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O31" s="14">
         <f t="shared" ca="1" si="1"/>
@@ -12571,23 +12571,23 @@
       </c>
       <c r="P31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="Q31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="R31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="S31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="T31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="U31" s="14">
         <f t="shared" ca="1" si="1"/>
@@ -12595,43 +12595,43 @@
       </c>
       <c r="V31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="W31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="Y31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="Z31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AA31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AB31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="AD31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AE31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="AF31" s="14">
         <f t="shared" ca="1" si="1"/>
@@ -12643,7 +12643,7 @@
       </c>
       <c r="AH31" s="14">
         <f ca="1">INT(ROUND(_xlfn.NORM.INV(RAND(), $C28,$C31),0))</f>
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.25">
@@ -12652,7 +12652,7 @@
       </c>
       <c r="F32" s="2">
         <f ca="1">MIN(E31:AH31)</f>
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
@@ -12661,7 +12661,7 @@
       </c>
       <c r="F33" s="15">
         <f ca="1">MAX(E31:AH31)</f>
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -12678,7 +12678,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A220B2A8-3D74-4185-A0A2-5AAD8496F6C6}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12697,13 +12699,13 @@
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -12714,21 +12716,21 @@
         <v>17</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>29</v>
@@ -12737,7 +12739,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>28</v>
@@ -12746,18 +12748,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new articles and updated logbook with data on the simulation employed by the Imperial College team
</commit_message>
<xml_diff>
--- a/assets/SIRD Model.xlsx
+++ b/assets/SIRD Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Task Stage\Task - covidsims\covidsims\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F2069F-2D9C-4DEA-B1F0-506765415224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E64E3D-54BD-4553-862A-550E1E823F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="38640" windowHeight="16440" tabRatio="659" activeTab="1" xr2:uid="{C9EED678-3558-4294-B636-EA4BD58922A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="659" activeTab="5" xr2:uid="{C9EED678-3558-4294-B636-EA4BD58922A2}"/>
   </bookViews>
   <sheets>
     <sheet name="SIRD model" sheetId="20" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="96">
   <si>
     <t>I(t)</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>∆R(t) = R(t) - R(t - 1)</t>
+  </si>
+  <si>
+    <t>https://www1.folha.uol.com.br/equilibrioesaude/2021/06/conheca-o-segredo-de-fernao-unica-cidade-de-sao-paulo-sem-morte-por-covid.shtml</t>
+  </si>
+  <si>
+    <t>Conheça o segredo de Fernão, única cidade de São Paulo sem morte por Covid - Município de menos de 2.000 habitantes aposta em medidas como monitoramento de casos e carro de som</t>
   </si>
 </sst>
 </file>
@@ -8365,7 +8371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E516D12-5BAB-48F7-A871-EC73412C1170}">
   <dimension ref="A8:AG20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -12536,7 +12542,7 @@
       </c>
       <c r="E31" s="14">
         <f ca="1">INT(ROUND(_xlfn.NORM.INV(RAND(), $C28,$C31),0))</f>
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F31" s="14">
         <f t="shared" ref="F31:AG31" ca="1" si="1">INT(ROUND(_xlfn.NORM.INV(RAND(), $C28,$C31),0))</f>
@@ -12544,79 +12550,79 @@
       </c>
       <c r="G31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="J31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="K31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="L31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="M31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="N31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="P31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="Q31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="T31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="U31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="V31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="W31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Y31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Z31" s="14">
         <f t="shared" ca="1" si="1"/>
@@ -12628,31 +12634,31 @@
       </c>
       <c r="AB31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="AC31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="AD31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="AE31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AF31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="AG31" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AH31" s="14">
         <f ca="1">INT(ROUND(_xlfn.NORM.INV(RAND(), $C28,$C31),0))</f>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.25">
@@ -12661,7 +12667,7 @@
       </c>
       <c r="F32" s="2">
         <f ca="1">MIN(E31:AH31)</f>
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
@@ -12670,7 +12676,7 @@
       </c>
       <c r="F33" s="15">
         <f ca="1">MAX(E31:AH31)</f>
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -12685,10 +12691,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A220B2A8-3D74-4185-A0A2-5AAD8496F6C6}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12774,6 +12780,14 @@
         <v>87</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F180FA8D-6669-4C5C-8CD4-B0C6032DF6F8}"/>
@@ -12782,6 +12796,7 @@
     <hyperlink ref="B5" r:id="rId4" xr:uid="{686789FA-7D85-4FD5-8CD9-403D9EB86CFF}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{8D8884B6-885B-4E38-BF72-2EDB8910415A}"/>
     <hyperlink ref="B8" r:id="rId6" xr:uid="{236C61C3-E49B-4049-801B-48A2FC1F670E}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{DF8935DB-BA16-4C97-9D82-D64E52EEBF24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>